<commit_message>
Update lai CDM và  PDM
Update lai CDM và  PDM
</commit_message>
<xml_diff>
--- a/Documents/Design/CDM+PDM.xlsx
+++ b/Documents/Design/CDM+PDM.xlsx
@@ -5,11 +5,11 @@
   <workbookPr defaultThemeVersion="153222"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\GIFHUB\QuanLiGiayKhaiSinh\Documents\Design\CDM and PDM\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\GIFHUB\QuanLiGiayKhaiSinh\Documents\Design\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="20490" windowHeight="7755"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="20490" windowHeight="7755" activeTab="2"/>
   </bookViews>
   <sheets>
     <sheet name="Lịch sử thay đổi" sheetId="1" r:id="rId1"/>
@@ -26,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="21" uniqueCount="15">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="23" uniqueCount="16">
   <si>
     <t>QUẢN LÍ KHAI SINH</t>
   </si>
@@ -72,6 +72,9 @@
   </si>
   <si>
     <t xml:space="preserve">UpLoad File </t>
+  </si>
+  <si>
+    <t>Update Lai CDM và PDM</t>
   </si>
 </sst>
 </file>
@@ -362,6 +365,9 @@
     <xf numFmtId="0" fontId="5" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
@@ -373,8 +379,8 @@
     <xf numFmtId="0" fontId="4" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
+    <xf numFmtId="14" fontId="2" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -392,9 +398,6 @@
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="14" fontId="2" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
   </cellXfs>
@@ -419,19 +422,19 @@
   <xdr:twoCellAnchor editAs="oneCell">
     <xdr:from>
       <xdr:col>0</xdr:col>
-      <xdr:colOff>609601</xdr:colOff>
-      <xdr:row>5</xdr:row>
-      <xdr:rowOff>38100</xdr:rowOff>
+      <xdr:colOff>885825</xdr:colOff>
+      <xdr:row>2</xdr:row>
+      <xdr:rowOff>152400</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>9</xdr:col>
-      <xdr:colOff>113507</xdr:colOff>
-      <xdr:row>25</xdr:row>
-      <xdr:rowOff>142875</xdr:rowOff>
+      <xdr:col>8</xdr:col>
+      <xdr:colOff>904876</xdr:colOff>
+      <xdr:row>37</xdr:row>
+      <xdr:rowOff>130786</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
-        <xdr:cNvPr id="3" name="Picture 2"/>
+        <xdr:cNvPr id="4" name="Picture 3"/>
         <xdr:cNvPicPr>
           <a:picLocks noChangeAspect="1" noChangeArrowheads="1"/>
         </xdr:cNvPicPr>
@@ -451,8 +454,8 @@
       </xdr:blipFill>
       <xdr:spPr bwMode="auto">
         <a:xfrm>
-          <a:off x="609601" y="1228725"/>
-          <a:ext cx="8590756" cy="3914775"/>
+          <a:off x="885825" y="771525"/>
+          <a:ext cx="8096251" cy="6645886"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -478,20 +481,20 @@
 <xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
   <xdr:twoCellAnchor editAs="oneCell">
     <xdr:from>
-      <xdr:col>0</xdr:col>
-      <xdr:colOff>428625</xdr:colOff>
+      <xdr:col>1</xdr:col>
+      <xdr:colOff>228600</xdr:colOff>
       <xdr:row>3</xdr:row>
-      <xdr:rowOff>123825</xdr:rowOff>
+      <xdr:rowOff>9525</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>11</xdr:col>
-      <xdr:colOff>323850</xdr:colOff>
-      <xdr:row>37</xdr:row>
-      <xdr:rowOff>171450</xdr:rowOff>
+      <xdr:col>9</xdr:col>
+      <xdr:colOff>847725</xdr:colOff>
+      <xdr:row>41</xdr:row>
+      <xdr:rowOff>57150</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
-        <xdr:cNvPr id="4" name="Picture 3"/>
+        <xdr:cNvPr id="5" name="Picture 4"/>
         <xdr:cNvPicPr>
           <a:picLocks noChangeAspect="1" noChangeArrowheads="1"/>
         </xdr:cNvPicPr>
@@ -511,8 +514,8 @@
       </xdr:blipFill>
       <xdr:spPr bwMode="auto">
         <a:xfrm>
-          <a:off x="428625" y="933450"/>
-          <a:ext cx="11001375" cy="6524625"/>
+          <a:off x="1238250" y="819150"/>
+          <a:ext cx="8696325" cy="7286625"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -799,7 +802,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:K15"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="G6" sqref="G6:K6"/>
     </sheetView>
   </sheetViews>
@@ -813,26 +816,26 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:11" s="2" customFormat="1" ht="25.5" x14ac:dyDescent="0.25">
-      <c r="A1" s="18" t="s">
+      <c r="A1" s="19" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="18"/>
-      <c r="C1" s="18"/>
-      <c r="D1" s="18"/>
-      <c r="E1" s="18"/>
-      <c r="F1" s="18"/>
-      <c r="G1" s="18"/>
-      <c r="H1" s="18"/>
-      <c r="I1" s="18"/>
-      <c r="J1" s="18"/>
+      <c r="B1" s="19"/>
+      <c r="C1" s="19"/>
+      <c r="D1" s="19"/>
+      <c r="E1" s="19"/>
+      <c r="F1" s="19"/>
+      <c r="G1" s="19"/>
+      <c r="H1" s="19"/>
+      <c r="I1" s="19"/>
+      <c r="J1" s="19"/>
       <c r="K1" s="1"/>
     </row>
     <row r="2" spans="1:11" s="2" customFormat="1" ht="25.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A2" s="19" t="s">
+      <c r="A2" s="20" t="s">
         <v>1</v>
       </c>
-      <c r="B2" s="19"/>
-      <c r="C2" s="19"/>
+      <c r="B2" s="20"/>
+      <c r="C2" s="20"/>
       <c r="D2" s="3"/>
       <c r="E2" s="3"/>
       <c r="F2" s="3"/>
@@ -846,229 +849,205 @@
       <c r="A3" s="5" t="s">
         <v>2</v>
       </c>
-      <c r="B3" s="20" t="s">
+      <c r="B3" s="21" t="s">
         <v>3</v>
       </c>
-      <c r="C3" s="20"/>
-      <c r="D3" s="20"/>
-      <c r="E3" s="20" t="s">
+      <c r="C3" s="21"/>
+      <c r="D3" s="21"/>
+      <c r="E3" s="21" t="s">
         <v>4</v>
       </c>
-      <c r="F3" s="20"/>
-      <c r="G3" s="20" t="s">
+      <c r="F3" s="21"/>
+      <c r="G3" s="21" t="s">
         <v>5</v>
       </c>
-      <c r="H3" s="20"/>
-      <c r="I3" s="20"/>
-      <c r="J3" s="20"/>
-      <c r="K3" s="20"/>
+      <c r="H3" s="21"/>
+      <c r="I3" s="21"/>
+      <c r="J3" s="21"/>
+      <c r="K3" s="21"/>
     </row>
     <row r="4" spans="1:11" ht="42.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A4" s="7">
         <v>1</v>
       </c>
-      <c r="B4" s="21" t="s">
+      <c r="B4" s="17" t="s">
         <v>12</v>
       </c>
-      <c r="C4" s="17"/>
-      <c r="D4" s="17"/>
-      <c r="E4" s="17" t="s">
+      <c r="C4" s="18"/>
+      <c r="D4" s="18"/>
+      <c r="E4" s="18" t="s">
         <v>6</v>
       </c>
-      <c r="F4" s="17"/>
-      <c r="G4" s="17" t="s">
+      <c r="F4" s="18"/>
+      <c r="G4" s="18" t="s">
         <v>7</v>
       </c>
-      <c r="H4" s="17"/>
-      <c r="I4" s="17"/>
-      <c r="J4" s="17"/>
-      <c r="K4" s="17"/>
+      <c r="H4" s="18"/>
+      <c r="I4" s="18"/>
+      <c r="J4" s="18"/>
+      <c r="K4" s="18"/>
     </row>
     <row r="5" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A5" s="7">
         <v>2</v>
       </c>
-      <c r="B5" s="17" t="s">
+      <c r="B5" s="18" t="s">
         <v>13</v>
       </c>
-      <c r="C5" s="17"/>
-      <c r="D5" s="17"/>
-      <c r="E5" s="28">
+      <c r="C5" s="18"/>
+      <c r="D5" s="18"/>
+      <c r="E5" s="22">
         <v>42825</v>
       </c>
-      <c r="F5" s="17"/>
-      <c r="G5" s="17" t="s">
+      <c r="F5" s="18"/>
+      <c r="G5" s="18" t="s">
         <v>14</v>
       </c>
-      <c r="H5" s="17"/>
-      <c r="I5" s="17"/>
-      <c r="J5" s="17"/>
-      <c r="K5" s="17"/>
+      <c r="H5" s="18"/>
+      <c r="I5" s="18"/>
+      <c r="J5" s="18"/>
+      <c r="K5" s="18"/>
     </row>
     <row r="6" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A6" s="7"/>
-      <c r="B6" s="17"/>
-      <c r="C6" s="17"/>
-      <c r="D6" s="17"/>
-      <c r="E6" s="17"/>
-      <c r="F6" s="17"/>
-      <c r="G6" s="17"/>
-      <c r="H6" s="17"/>
-      <c r="I6" s="17"/>
-      <c r="J6" s="17"/>
-      <c r="K6" s="17"/>
+      <c r="A6" s="7">
+        <v>3</v>
+      </c>
+      <c r="B6" s="18" t="s">
+        <v>13</v>
+      </c>
+      <c r="C6" s="18"/>
+      <c r="D6" s="18"/>
+      <c r="E6" s="22">
+        <v>42828</v>
+      </c>
+      <c r="F6" s="18"/>
+      <c r="G6" s="18" t="s">
+        <v>15</v>
+      </c>
+      <c r="H6" s="18"/>
+      <c r="I6" s="18"/>
+      <c r="J6" s="18"/>
+      <c r="K6" s="18"/>
     </row>
     <row r="7" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A7" s="7"/>
-      <c r="B7" s="17"/>
-      <c r="C7" s="17"/>
-      <c r="D7" s="17"/>
-      <c r="E7" s="17"/>
-      <c r="F7" s="17"/>
-      <c r="G7" s="17"/>
-      <c r="H7" s="17"/>
-      <c r="I7" s="17"/>
-      <c r="J7" s="17"/>
-      <c r="K7" s="17"/>
+      <c r="B7" s="18"/>
+      <c r="C7" s="18"/>
+      <c r="D7" s="18"/>
+      <c r="E7" s="18"/>
+      <c r="F7" s="18"/>
+      <c r="G7" s="18"/>
+      <c r="H7" s="18"/>
+      <c r="I7" s="18"/>
+      <c r="J7" s="18"/>
+      <c r="K7" s="18"/>
     </row>
     <row r="8" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A8" s="7"/>
-      <c r="B8" s="17"/>
-      <c r="C8" s="17"/>
-      <c r="D8" s="17"/>
-      <c r="E8" s="17"/>
-      <c r="F8" s="17"/>
-      <c r="G8" s="17"/>
-      <c r="H8" s="17"/>
-      <c r="I8" s="17"/>
-      <c r="J8" s="17"/>
-      <c r="K8" s="17"/>
+      <c r="B8" s="18"/>
+      <c r="C8" s="18"/>
+      <c r="D8" s="18"/>
+      <c r="E8" s="18"/>
+      <c r="F8" s="18"/>
+      <c r="G8" s="18"/>
+      <c r="H8" s="18"/>
+      <c r="I8" s="18"/>
+      <c r="J8" s="18"/>
+      <c r="K8" s="18"/>
     </row>
     <row r="9" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A9" s="7"/>
-      <c r="B9" s="17"/>
-      <c r="C9" s="17"/>
-      <c r="D9" s="17"/>
-      <c r="E9" s="17"/>
-      <c r="F9" s="17"/>
-      <c r="G9" s="17"/>
-      <c r="H9" s="17"/>
-      <c r="I9" s="17"/>
-      <c r="J9" s="17"/>
-      <c r="K9" s="17"/>
+      <c r="B9" s="18"/>
+      <c r="C9" s="18"/>
+      <c r="D9" s="18"/>
+      <c r="E9" s="18"/>
+      <c r="F9" s="18"/>
+      <c r="G9" s="18"/>
+      <c r="H9" s="18"/>
+      <c r="I9" s="18"/>
+      <c r="J9" s="18"/>
+      <c r="K9" s="18"/>
     </row>
     <row r="10" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A10" s="7"/>
-      <c r="B10" s="17"/>
-      <c r="C10" s="17"/>
-      <c r="D10" s="17"/>
-      <c r="E10" s="17"/>
-      <c r="F10" s="17"/>
-      <c r="G10" s="17"/>
-      <c r="H10" s="17"/>
-      <c r="I10" s="17"/>
-      <c r="J10" s="17"/>
-      <c r="K10" s="17"/>
+      <c r="B10" s="18"/>
+      <c r="C10" s="18"/>
+      <c r="D10" s="18"/>
+      <c r="E10" s="18"/>
+      <c r="F10" s="18"/>
+      <c r="G10" s="18"/>
+      <c r="H10" s="18"/>
+      <c r="I10" s="18"/>
+      <c r="J10" s="18"/>
+      <c r="K10" s="18"/>
     </row>
     <row r="11" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A11" s="7"/>
-      <c r="B11" s="17"/>
-      <c r="C11" s="17"/>
-      <c r="D11" s="17"/>
-      <c r="E11" s="17"/>
-      <c r="F11" s="17"/>
-      <c r="G11" s="17"/>
-      <c r="H11" s="17"/>
-      <c r="I11" s="17"/>
-      <c r="J11" s="17"/>
-      <c r="K11" s="17"/>
+      <c r="B11" s="18"/>
+      <c r="C11" s="18"/>
+      <c r="D11" s="18"/>
+      <c r="E11" s="18"/>
+      <c r="F11" s="18"/>
+      <c r="G11" s="18"/>
+      <c r="H11" s="18"/>
+      <c r="I11" s="18"/>
+      <c r="J11" s="18"/>
+      <c r="K11" s="18"/>
     </row>
     <row r="12" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A12" s="7"/>
-      <c r="B12" s="17"/>
-      <c r="C12" s="17"/>
-      <c r="D12" s="17"/>
-      <c r="E12" s="17"/>
-      <c r="F12" s="17"/>
-      <c r="G12" s="17"/>
-      <c r="H12" s="17"/>
-      <c r="I12" s="17"/>
-      <c r="J12" s="17"/>
-      <c r="K12" s="17"/>
+      <c r="B12" s="18"/>
+      <c r="C12" s="18"/>
+      <c r="D12" s="18"/>
+      <c r="E12" s="18"/>
+      <c r="F12" s="18"/>
+      <c r="G12" s="18"/>
+      <c r="H12" s="18"/>
+      <c r="I12" s="18"/>
+      <c r="J12" s="18"/>
+      <c r="K12" s="18"/>
     </row>
     <row r="13" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A13" s="7"/>
-      <c r="B13" s="17"/>
-      <c r="C13" s="17"/>
-      <c r="D13" s="17"/>
-      <c r="E13" s="17"/>
-      <c r="F13" s="17"/>
-      <c r="G13" s="17"/>
-      <c r="H13" s="17"/>
-      <c r="I13" s="17"/>
-      <c r="J13" s="17"/>
-      <c r="K13" s="17"/>
+      <c r="B13" s="18"/>
+      <c r="C13" s="18"/>
+      <c r="D13" s="18"/>
+      <c r="E13" s="18"/>
+      <c r="F13" s="18"/>
+      <c r="G13" s="18"/>
+      <c r="H13" s="18"/>
+      <c r="I13" s="18"/>
+      <c r="J13" s="18"/>
+      <c r="K13" s="18"/>
     </row>
     <row r="14" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A14" s="7"/>
-      <c r="B14" s="17"/>
-      <c r="C14" s="17"/>
-      <c r="D14" s="17"/>
-      <c r="E14" s="17"/>
-      <c r="F14" s="17"/>
-      <c r="G14" s="17"/>
-      <c r="H14" s="17"/>
-      <c r="I14" s="17"/>
-      <c r="J14" s="17"/>
-      <c r="K14" s="17"/>
+      <c r="B14" s="18"/>
+      <c r="C14" s="18"/>
+      <c r="D14" s="18"/>
+      <c r="E14" s="18"/>
+      <c r="F14" s="18"/>
+      <c r="G14" s="18"/>
+      <c r="H14" s="18"/>
+      <c r="I14" s="18"/>
+      <c r="J14" s="18"/>
+      <c r="K14" s="18"/>
     </row>
     <row r="15" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A15" s="7"/>
-      <c r="B15" s="17"/>
-      <c r="C15" s="17"/>
-      <c r="D15" s="17"/>
-      <c r="E15" s="17"/>
-      <c r="F15" s="17"/>
-      <c r="G15" s="17"/>
-      <c r="H15" s="17"/>
-      <c r="I15" s="17"/>
-      <c r="J15" s="17"/>
-      <c r="K15" s="17"/>
+      <c r="B15" s="18"/>
+      <c r="C15" s="18"/>
+      <c r="D15" s="18"/>
+      <c r="E15" s="18"/>
+      <c r="F15" s="18"/>
+      <c r="G15" s="18"/>
+      <c r="H15" s="18"/>
+      <c r="I15" s="18"/>
+      <c r="J15" s="18"/>
+      <c r="K15" s="18"/>
     </row>
   </sheetData>
   <mergeCells count="41">
-    <mergeCell ref="B4:D4"/>
-    <mergeCell ref="E4:F4"/>
-    <mergeCell ref="G4:K4"/>
-    <mergeCell ref="A1:J1"/>
-    <mergeCell ref="A2:C2"/>
-    <mergeCell ref="B3:D3"/>
-    <mergeCell ref="E3:F3"/>
-    <mergeCell ref="G3:K3"/>
-    <mergeCell ref="B5:D5"/>
-    <mergeCell ref="E5:F5"/>
-    <mergeCell ref="G5:K5"/>
-    <mergeCell ref="B6:D6"/>
-    <mergeCell ref="E6:F6"/>
-    <mergeCell ref="G6:K6"/>
-    <mergeCell ref="B7:D7"/>
-    <mergeCell ref="E7:F7"/>
-    <mergeCell ref="G7:K7"/>
-    <mergeCell ref="B8:D8"/>
-    <mergeCell ref="E8:F8"/>
-    <mergeCell ref="G8:K8"/>
-    <mergeCell ref="B9:D9"/>
-    <mergeCell ref="E9:F9"/>
-    <mergeCell ref="G9:K9"/>
-    <mergeCell ref="B10:D10"/>
-    <mergeCell ref="E10:F10"/>
-    <mergeCell ref="G10:K10"/>
-    <mergeCell ref="B11:D11"/>
-    <mergeCell ref="E11:F11"/>
-    <mergeCell ref="G11:K11"/>
-    <mergeCell ref="B12:D12"/>
-    <mergeCell ref="E12:F12"/>
-    <mergeCell ref="G12:K12"/>
     <mergeCell ref="B15:D15"/>
     <mergeCell ref="E15:F15"/>
     <mergeCell ref="G15:K15"/>
@@ -1078,6 +1057,38 @@
     <mergeCell ref="B14:D14"/>
     <mergeCell ref="E14:F14"/>
     <mergeCell ref="G14:K14"/>
+    <mergeCell ref="B11:D11"/>
+    <mergeCell ref="E11:F11"/>
+    <mergeCell ref="G11:K11"/>
+    <mergeCell ref="B12:D12"/>
+    <mergeCell ref="E12:F12"/>
+    <mergeCell ref="G12:K12"/>
+    <mergeCell ref="B9:D9"/>
+    <mergeCell ref="E9:F9"/>
+    <mergeCell ref="G9:K9"/>
+    <mergeCell ref="B10:D10"/>
+    <mergeCell ref="E10:F10"/>
+    <mergeCell ref="G10:K10"/>
+    <mergeCell ref="B7:D7"/>
+    <mergeCell ref="E7:F7"/>
+    <mergeCell ref="G7:K7"/>
+    <mergeCell ref="B8:D8"/>
+    <mergeCell ref="E8:F8"/>
+    <mergeCell ref="G8:K8"/>
+    <mergeCell ref="B5:D5"/>
+    <mergeCell ref="E5:F5"/>
+    <mergeCell ref="G5:K5"/>
+    <mergeCell ref="B6:D6"/>
+    <mergeCell ref="E6:F6"/>
+    <mergeCell ref="G6:K6"/>
+    <mergeCell ref="B4:D4"/>
+    <mergeCell ref="E4:F4"/>
+    <mergeCell ref="G4:K4"/>
+    <mergeCell ref="A1:J1"/>
+    <mergeCell ref="A2:C2"/>
+    <mergeCell ref="B3:D3"/>
+    <mergeCell ref="E3:F3"/>
+    <mergeCell ref="G3:K3"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -1087,8 +1098,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:AQ130"/>
   <sheetViews>
-    <sheetView topLeftCell="A16" workbookViewId="0">
-      <selection activeCell="E38" sqref="E38"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="J19" sqref="J19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="15.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1099,33 +1110,33 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:11" ht="26.25" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A1" s="22" t="s">
+      <c r="A1" s="23" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="22"/>
-      <c r="C1" s="22"/>
-      <c r="D1" s="22"/>
-      <c r="E1" s="22"/>
-      <c r="F1" s="22"/>
-      <c r="G1" s="22"/>
-      <c r="H1" s="22"/>
-      <c r="I1" s="22"/>
-      <c r="J1" s="22"/>
+      <c r="B1" s="23"/>
+      <c r="C1" s="23"/>
+      <c r="D1" s="23"/>
+      <c r="E1" s="23"/>
+      <c r="F1" s="23"/>
+      <c r="G1" s="23"/>
+      <c r="H1" s="23"/>
+      <c r="I1" s="23"/>
+      <c r="J1" s="23"/>
       <c r="K1" s="3"/>
     </row>
     <row r="2" spans="1:11" ht="22.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A2" s="23" t="s">
+      <c r="A2" s="24" t="s">
         <v>8</v>
       </c>
-      <c r="B2" s="24"/>
-      <c r="C2" s="25" t="s">
+      <c r="B2" s="25"/>
+      <c r="C2" s="26" t="s">
         <v>10</v>
       </c>
-      <c r="D2" s="26"/>
-      <c r="E2" s="26"/>
-      <c r="F2" s="26"/>
-      <c r="G2" s="26"/>
-      <c r="H2" s="27"/>
+      <c r="D2" s="27"/>
+      <c r="E2" s="27"/>
+      <c r="F2" s="27"/>
+      <c r="G2" s="27"/>
+      <c r="H2" s="28"/>
       <c r="I2" s="11" t="s">
         <v>9</v>
       </c>
@@ -2775,8 +2786,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:AS137"/>
   <sheetViews>
-    <sheetView topLeftCell="A34" workbookViewId="0">
-      <selection activeCell="H42" sqref="H42"/>
+    <sheetView tabSelected="1" topLeftCell="A13" workbookViewId="0">
+      <selection activeCell="A4" sqref="A4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="15.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2787,37 +2798,37 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:13" ht="26.25" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A1" s="22" t="s">
+      <c r="A1" s="23" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="22"/>
-      <c r="C1" s="22"/>
-      <c r="D1" s="22"/>
-      <c r="E1" s="22"/>
-      <c r="F1" s="22"/>
-      <c r="G1" s="22"/>
-      <c r="H1" s="22"/>
-      <c r="I1" s="22"/>
-      <c r="J1" s="22"/>
-      <c r="K1" s="22"/>
-      <c r="L1" s="22"/>
+      <c r="B1" s="23"/>
+      <c r="C1" s="23"/>
+      <c r="D1" s="23"/>
+      <c r="E1" s="23"/>
+      <c r="F1" s="23"/>
+      <c r="G1" s="23"/>
+      <c r="H1" s="23"/>
+      <c r="I1" s="23"/>
+      <c r="J1" s="23"/>
+      <c r="K1" s="23"/>
+      <c r="L1" s="23"/>
       <c r="M1" s="3"/>
     </row>
     <row r="2" spans="1:13" ht="22.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A2" s="23" t="s">
+      <c r="A2" s="24" t="s">
         <v>8</v>
       </c>
-      <c r="B2" s="24"/>
-      <c r="C2" s="25" t="s">
+      <c r="B2" s="25"/>
+      <c r="C2" s="26" t="s">
         <v>11</v>
       </c>
-      <c r="D2" s="26"/>
-      <c r="E2" s="26"/>
-      <c r="F2" s="26"/>
-      <c r="G2" s="26"/>
-      <c r="H2" s="26"/>
-      <c r="I2" s="26"/>
-      <c r="J2" s="27"/>
+      <c r="D2" s="27"/>
+      <c r="E2" s="27"/>
+      <c r="F2" s="27"/>
+      <c r="G2" s="27"/>
+      <c r="H2" s="27"/>
+      <c r="I2" s="27"/>
+      <c r="J2" s="28"/>
       <c r="K2" s="11" t="s">
         <v>9</v>
       </c>

</xml_diff>

<commit_message>
update CDM và PDM
Update CDM và PDM
</commit_message>
<xml_diff>
--- a/Documents/Design/CDM+PDM.xlsx
+++ b/Documents/Design/CDM+PDM.xlsx
@@ -365,10 +365,13 @@
     <xf numFmtId="0" fontId="5" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="14" fontId="2" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
+      <alignment horizontal="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -377,9 +380,6 @@
       <alignment horizontal="left" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="14" fontId="2" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -422,19 +422,19 @@
   <xdr:twoCellAnchor editAs="oneCell">
     <xdr:from>
       <xdr:col>0</xdr:col>
-      <xdr:colOff>885825</xdr:colOff>
+      <xdr:colOff>733426</xdr:colOff>
       <xdr:row>2</xdr:row>
-      <xdr:rowOff>152400</xdr:rowOff>
+      <xdr:rowOff>161925</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>8</xdr:col>
-      <xdr:colOff>904876</xdr:colOff>
-      <xdr:row>37</xdr:row>
-      <xdr:rowOff>130786</xdr:rowOff>
+      <xdr:colOff>523876</xdr:colOff>
+      <xdr:row>38</xdr:row>
+      <xdr:rowOff>37883</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
-        <xdr:cNvPr id="4" name="Picture 3"/>
+        <xdr:cNvPr id="3" name="Picture 2"/>
         <xdr:cNvPicPr>
           <a:picLocks noChangeAspect="1" noChangeArrowheads="1"/>
         </xdr:cNvPicPr>
@@ -454,8 +454,8 @@
       </xdr:blipFill>
       <xdr:spPr bwMode="auto">
         <a:xfrm>
-          <a:off x="885825" y="771525"/>
-          <a:ext cx="8096251" cy="6645886"/>
+          <a:off x="733426" y="781050"/>
+          <a:ext cx="7867650" cy="6733958"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -481,20 +481,20 @@
 <xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
   <xdr:twoCellAnchor editAs="oneCell">
     <xdr:from>
-      <xdr:col>1</xdr:col>
-      <xdr:colOff>228600</xdr:colOff>
+      <xdr:col>2</xdr:col>
+      <xdr:colOff>38100</xdr:colOff>
       <xdr:row>3</xdr:row>
-      <xdr:rowOff>9525</xdr:rowOff>
+      <xdr:rowOff>19050</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>9</xdr:col>
-      <xdr:colOff>847725</xdr:colOff>
+      <xdr:col>10</xdr:col>
+      <xdr:colOff>657225</xdr:colOff>
       <xdr:row>41</xdr:row>
-      <xdr:rowOff>57150</xdr:rowOff>
+      <xdr:rowOff>66675</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
-        <xdr:cNvPr id="5" name="Picture 4"/>
+        <xdr:cNvPr id="3" name="Picture 2"/>
         <xdr:cNvPicPr>
           <a:picLocks noChangeAspect="1" noChangeArrowheads="1"/>
         </xdr:cNvPicPr>
@@ -514,7 +514,7 @@
       </xdr:blipFill>
       <xdr:spPr bwMode="auto">
         <a:xfrm>
-          <a:off x="1238250" y="819150"/>
+          <a:off x="2057400" y="828675"/>
           <a:ext cx="8696325" cy="7286625"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
@@ -816,26 +816,26 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:11" s="2" customFormat="1" ht="25.5" x14ac:dyDescent="0.25">
-      <c r="A1" s="19" t="s">
+      <c r="A1" s="20" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="19"/>
-      <c r="C1" s="19"/>
-      <c r="D1" s="19"/>
-      <c r="E1" s="19"/>
-      <c r="F1" s="19"/>
-      <c r="G1" s="19"/>
-      <c r="H1" s="19"/>
-      <c r="I1" s="19"/>
-      <c r="J1" s="19"/>
+      <c r="B1" s="20"/>
+      <c r="C1" s="20"/>
+      <c r="D1" s="20"/>
+      <c r="E1" s="20"/>
+      <c r="F1" s="20"/>
+      <c r="G1" s="20"/>
+      <c r="H1" s="20"/>
+      <c r="I1" s="20"/>
+      <c r="J1" s="20"/>
       <c r="K1" s="1"/>
     </row>
     <row r="2" spans="1:11" s="2" customFormat="1" ht="25.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A2" s="20" t="s">
+      <c r="A2" s="21" t="s">
         <v>1</v>
       </c>
-      <c r="B2" s="20"/>
-      <c r="C2" s="20"/>
+      <c r="B2" s="21"/>
+      <c r="C2" s="21"/>
       <c r="D2" s="3"/>
       <c r="E2" s="3"/>
       <c r="F2" s="3"/>
@@ -849,205 +849,237 @@
       <c r="A3" s="5" t="s">
         <v>2</v>
       </c>
-      <c r="B3" s="21" t="s">
+      <c r="B3" s="22" t="s">
         <v>3</v>
       </c>
-      <c r="C3" s="21"/>
-      <c r="D3" s="21"/>
-      <c r="E3" s="21" t="s">
+      <c r="C3" s="22"/>
+      <c r="D3" s="22"/>
+      <c r="E3" s="22" t="s">
         <v>4</v>
       </c>
-      <c r="F3" s="21"/>
-      <c r="G3" s="21" t="s">
+      <c r="F3" s="22"/>
+      <c r="G3" s="22" t="s">
         <v>5</v>
       </c>
-      <c r="H3" s="21"/>
-      <c r="I3" s="21"/>
-      <c r="J3" s="21"/>
-      <c r="K3" s="21"/>
+      <c r="H3" s="22"/>
+      <c r="I3" s="22"/>
+      <c r="J3" s="22"/>
+      <c r="K3" s="22"/>
     </row>
     <row r="4" spans="1:11" ht="42.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A4" s="7">
         <v>1</v>
       </c>
-      <c r="B4" s="17" t="s">
+      <c r="B4" s="19" t="s">
         <v>12</v>
       </c>
-      <c r="C4" s="18"/>
-      <c r="D4" s="18"/>
-      <c r="E4" s="18" t="s">
+      <c r="C4" s="17"/>
+      <c r="D4" s="17"/>
+      <c r="E4" s="17" t="s">
         <v>6</v>
       </c>
-      <c r="F4" s="18"/>
-      <c r="G4" s="18" t="s">
+      <c r="F4" s="17"/>
+      <c r="G4" s="17" t="s">
         <v>7</v>
       </c>
-      <c r="H4" s="18"/>
-      <c r="I4" s="18"/>
-      <c r="J4" s="18"/>
-      <c r="K4" s="18"/>
+      <c r="H4" s="17"/>
+      <c r="I4" s="17"/>
+      <c r="J4" s="17"/>
+      <c r="K4" s="17"/>
     </row>
     <row r="5" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A5" s="7">
         <v>2</v>
       </c>
-      <c r="B5" s="18" t="s">
+      <c r="B5" s="17" t="s">
         <v>13</v>
       </c>
-      <c r="C5" s="18"/>
-      <c r="D5" s="18"/>
-      <c r="E5" s="22">
+      <c r="C5" s="17"/>
+      <c r="D5" s="17"/>
+      <c r="E5" s="18">
         <v>42825</v>
       </c>
-      <c r="F5" s="18"/>
-      <c r="G5" s="18" t="s">
+      <c r="F5" s="17"/>
+      <c r="G5" s="17" t="s">
         <v>14</v>
       </c>
-      <c r="H5" s="18"/>
-      <c r="I5" s="18"/>
-      <c r="J5" s="18"/>
-      <c r="K5" s="18"/>
+      <c r="H5" s="17"/>
+      <c r="I5" s="17"/>
+      <c r="J5" s="17"/>
+      <c r="K5" s="17"/>
     </row>
     <row r="6" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A6" s="7">
         <v>3</v>
       </c>
-      <c r="B6" s="18" t="s">
+      <c r="B6" s="17" t="s">
         <v>13</v>
       </c>
-      <c r="C6" s="18"/>
-      <c r="D6" s="18"/>
-      <c r="E6" s="22">
+      <c r="C6" s="17"/>
+      <c r="D6" s="17"/>
+      <c r="E6" s="18">
         <v>42828</v>
       </c>
-      <c r="F6" s="18"/>
-      <c r="G6" s="18" t="s">
+      <c r="F6" s="17"/>
+      <c r="G6" s="17" t="s">
         <v>15</v>
       </c>
-      <c r="H6" s="18"/>
-      <c r="I6" s="18"/>
-      <c r="J6" s="18"/>
-      <c r="K6" s="18"/>
+      <c r="H6" s="17"/>
+      <c r="I6" s="17"/>
+      <c r="J6" s="17"/>
+      <c r="K6" s="17"/>
     </row>
     <row r="7" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A7" s="7"/>
-      <c r="B7" s="18"/>
-      <c r="C7" s="18"/>
-      <c r="D7" s="18"/>
-      <c r="E7" s="18"/>
-      <c r="F7" s="18"/>
-      <c r="G7" s="18"/>
-      <c r="H7" s="18"/>
-      <c r="I7" s="18"/>
-      <c r="J7" s="18"/>
-      <c r="K7" s="18"/>
+      <c r="B7" s="17"/>
+      <c r="C7" s="17"/>
+      <c r="D7" s="17"/>
+      <c r="E7" s="17"/>
+      <c r="F7" s="17"/>
+      <c r="G7" s="17"/>
+      <c r="H7" s="17"/>
+      <c r="I7" s="17"/>
+      <c r="J7" s="17"/>
+      <c r="K7" s="17"/>
     </row>
     <row r="8" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A8" s="7"/>
-      <c r="B8" s="18"/>
-      <c r="C8" s="18"/>
-      <c r="D8" s="18"/>
-      <c r="E8" s="18"/>
-      <c r="F8" s="18"/>
-      <c r="G8" s="18"/>
-      <c r="H8" s="18"/>
-      <c r="I8" s="18"/>
-      <c r="J8" s="18"/>
-      <c r="K8" s="18"/>
+      <c r="B8" s="17"/>
+      <c r="C8" s="17"/>
+      <c r="D8" s="17"/>
+      <c r="E8" s="17"/>
+      <c r="F8" s="17"/>
+      <c r="G8" s="17"/>
+      <c r="H8" s="17"/>
+      <c r="I8" s="17"/>
+      <c r="J8" s="17"/>
+      <c r="K8" s="17"/>
     </row>
     <row r="9" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A9" s="7"/>
-      <c r="B9" s="18"/>
-      <c r="C9" s="18"/>
-      <c r="D9" s="18"/>
-      <c r="E9" s="18"/>
-      <c r="F9" s="18"/>
-      <c r="G9" s="18"/>
-      <c r="H9" s="18"/>
-      <c r="I9" s="18"/>
-      <c r="J9" s="18"/>
-      <c r="K9" s="18"/>
+      <c r="B9" s="17"/>
+      <c r="C9" s="17"/>
+      <c r="D9" s="17"/>
+      <c r="E9" s="17"/>
+      <c r="F9" s="17"/>
+      <c r="G9" s="17"/>
+      <c r="H9" s="17"/>
+      <c r="I9" s="17"/>
+      <c r="J9" s="17"/>
+      <c r="K9" s="17"/>
     </row>
     <row r="10" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A10" s="7"/>
-      <c r="B10" s="18"/>
-      <c r="C10" s="18"/>
-      <c r="D10" s="18"/>
-      <c r="E10" s="18"/>
-      <c r="F10" s="18"/>
-      <c r="G10" s="18"/>
-      <c r="H10" s="18"/>
-      <c r="I10" s="18"/>
-      <c r="J10" s="18"/>
-      <c r="K10" s="18"/>
+      <c r="B10" s="17"/>
+      <c r="C10" s="17"/>
+      <c r="D10" s="17"/>
+      <c r="E10" s="17"/>
+      <c r="F10" s="17"/>
+      <c r="G10" s="17"/>
+      <c r="H10" s="17"/>
+      <c r="I10" s="17"/>
+      <c r="J10" s="17"/>
+      <c r="K10" s="17"/>
     </row>
     <row r="11" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A11" s="7"/>
-      <c r="B11" s="18"/>
-      <c r="C11" s="18"/>
-      <c r="D11" s="18"/>
-      <c r="E11" s="18"/>
-      <c r="F11" s="18"/>
-      <c r="G11" s="18"/>
-      <c r="H11" s="18"/>
-      <c r="I11" s="18"/>
-      <c r="J11" s="18"/>
-      <c r="K11" s="18"/>
+      <c r="B11" s="17"/>
+      <c r="C11" s="17"/>
+      <c r="D11" s="17"/>
+      <c r="E11" s="17"/>
+      <c r="F11" s="17"/>
+      <c r="G11" s="17"/>
+      <c r="H11" s="17"/>
+      <c r="I11" s="17"/>
+      <c r="J11" s="17"/>
+      <c r="K11" s="17"/>
     </row>
     <row r="12" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A12" s="7"/>
-      <c r="B12" s="18"/>
-      <c r="C12" s="18"/>
-      <c r="D12" s="18"/>
-      <c r="E12" s="18"/>
-      <c r="F12" s="18"/>
-      <c r="G12" s="18"/>
-      <c r="H12" s="18"/>
-      <c r="I12" s="18"/>
-      <c r="J12" s="18"/>
-      <c r="K12" s="18"/>
+      <c r="B12" s="17"/>
+      <c r="C12" s="17"/>
+      <c r="D12" s="17"/>
+      <c r="E12" s="17"/>
+      <c r="F12" s="17"/>
+      <c r="G12" s="17"/>
+      <c r="H12" s="17"/>
+      <c r="I12" s="17"/>
+      <c r="J12" s="17"/>
+      <c r="K12" s="17"/>
     </row>
     <row r="13" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A13" s="7"/>
-      <c r="B13" s="18"/>
-      <c r="C13" s="18"/>
-      <c r="D13" s="18"/>
-      <c r="E13" s="18"/>
-      <c r="F13" s="18"/>
-      <c r="G13" s="18"/>
-      <c r="H13" s="18"/>
-      <c r="I13" s="18"/>
-      <c r="J13" s="18"/>
-      <c r="K13" s="18"/>
+      <c r="B13" s="17"/>
+      <c r="C13" s="17"/>
+      <c r="D13" s="17"/>
+      <c r="E13" s="17"/>
+      <c r="F13" s="17"/>
+      <c r="G13" s="17"/>
+      <c r="H13" s="17"/>
+      <c r="I13" s="17"/>
+      <c r="J13" s="17"/>
+      <c r="K13" s="17"/>
     </row>
     <row r="14" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A14" s="7"/>
-      <c r="B14" s="18"/>
-      <c r="C14" s="18"/>
-      <c r="D14" s="18"/>
-      <c r="E14" s="18"/>
-      <c r="F14" s="18"/>
-      <c r="G14" s="18"/>
-      <c r="H14" s="18"/>
-      <c r="I14" s="18"/>
-      <c r="J14" s="18"/>
-      <c r="K14" s="18"/>
+      <c r="B14" s="17"/>
+      <c r="C14" s="17"/>
+      <c r="D14" s="17"/>
+      <c r="E14" s="17"/>
+      <c r="F14" s="17"/>
+      <c r="G14" s="17"/>
+      <c r="H14" s="17"/>
+      <c r="I14" s="17"/>
+      <c r="J14" s="17"/>
+      <c r="K14" s="17"/>
     </row>
     <row r="15" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A15" s="7"/>
-      <c r="B15" s="18"/>
-      <c r="C15" s="18"/>
-      <c r="D15" s="18"/>
-      <c r="E15" s="18"/>
-      <c r="F15" s="18"/>
-      <c r="G15" s="18"/>
-      <c r="H15" s="18"/>
-      <c r="I15" s="18"/>
-      <c r="J15" s="18"/>
-      <c r="K15" s="18"/>
+      <c r="B15" s="17"/>
+      <c r="C15" s="17"/>
+      <c r="D15" s="17"/>
+      <c r="E15" s="17"/>
+      <c r="F15" s="17"/>
+      <c r="G15" s="17"/>
+      <c r="H15" s="17"/>
+      <c r="I15" s="17"/>
+      <c r="J15" s="17"/>
+      <c r="K15" s="17"/>
     </row>
   </sheetData>
   <mergeCells count="41">
+    <mergeCell ref="B4:D4"/>
+    <mergeCell ref="E4:F4"/>
+    <mergeCell ref="G4:K4"/>
+    <mergeCell ref="A1:J1"/>
+    <mergeCell ref="A2:C2"/>
+    <mergeCell ref="B3:D3"/>
+    <mergeCell ref="E3:F3"/>
+    <mergeCell ref="G3:K3"/>
+    <mergeCell ref="B5:D5"/>
+    <mergeCell ref="E5:F5"/>
+    <mergeCell ref="G5:K5"/>
+    <mergeCell ref="B6:D6"/>
+    <mergeCell ref="E6:F6"/>
+    <mergeCell ref="G6:K6"/>
+    <mergeCell ref="B7:D7"/>
+    <mergeCell ref="E7:F7"/>
+    <mergeCell ref="G7:K7"/>
+    <mergeCell ref="B8:D8"/>
+    <mergeCell ref="E8:F8"/>
+    <mergeCell ref="G8:K8"/>
+    <mergeCell ref="B9:D9"/>
+    <mergeCell ref="E9:F9"/>
+    <mergeCell ref="G9:K9"/>
+    <mergeCell ref="B10:D10"/>
+    <mergeCell ref="E10:F10"/>
+    <mergeCell ref="G10:K10"/>
+    <mergeCell ref="B11:D11"/>
+    <mergeCell ref="E11:F11"/>
+    <mergeCell ref="G11:K11"/>
+    <mergeCell ref="B12:D12"/>
+    <mergeCell ref="E12:F12"/>
+    <mergeCell ref="G12:K12"/>
     <mergeCell ref="B15:D15"/>
     <mergeCell ref="E15:F15"/>
     <mergeCell ref="G15:K15"/>
@@ -1057,38 +1089,6 @@
     <mergeCell ref="B14:D14"/>
     <mergeCell ref="E14:F14"/>
     <mergeCell ref="G14:K14"/>
-    <mergeCell ref="B11:D11"/>
-    <mergeCell ref="E11:F11"/>
-    <mergeCell ref="G11:K11"/>
-    <mergeCell ref="B12:D12"/>
-    <mergeCell ref="E12:F12"/>
-    <mergeCell ref="G12:K12"/>
-    <mergeCell ref="B9:D9"/>
-    <mergeCell ref="E9:F9"/>
-    <mergeCell ref="G9:K9"/>
-    <mergeCell ref="B10:D10"/>
-    <mergeCell ref="E10:F10"/>
-    <mergeCell ref="G10:K10"/>
-    <mergeCell ref="B7:D7"/>
-    <mergeCell ref="E7:F7"/>
-    <mergeCell ref="G7:K7"/>
-    <mergeCell ref="B8:D8"/>
-    <mergeCell ref="E8:F8"/>
-    <mergeCell ref="G8:K8"/>
-    <mergeCell ref="B5:D5"/>
-    <mergeCell ref="E5:F5"/>
-    <mergeCell ref="G5:K5"/>
-    <mergeCell ref="B6:D6"/>
-    <mergeCell ref="E6:F6"/>
-    <mergeCell ref="G6:K6"/>
-    <mergeCell ref="B4:D4"/>
-    <mergeCell ref="E4:F4"/>
-    <mergeCell ref="G4:K4"/>
-    <mergeCell ref="A1:J1"/>
-    <mergeCell ref="A2:C2"/>
-    <mergeCell ref="B3:D3"/>
-    <mergeCell ref="E3:F3"/>
-    <mergeCell ref="G3:K3"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -1098,8 +1098,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:AQ130"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="J19" sqref="J19"/>
+    <sheetView topLeftCell="A3" workbookViewId="0">
+      <selection activeCell="J35" sqref="J35"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="15.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2786,7 +2786,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:AS137"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A13" workbookViewId="0">
+    <sheetView tabSelected="1" workbookViewId="0">
       <selection activeCell="A4" sqref="A4"/>
     </sheetView>
   </sheetViews>

</xml_diff>

<commit_message>
update CDM va PDM
update CDM va PDM
</commit_message>
<xml_diff>
--- a/Documents/Design/CDM+PDM.xlsx
+++ b/Documents/Design/CDM+PDM.xlsx
@@ -365,10 +365,13 @@
     <xf numFmtId="0" fontId="5" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="14" fontId="2" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
+      <alignment horizontal="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -377,9 +380,6 @@
       <alignment horizontal="left" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="14" fontId="2" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -428,13 +428,13 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>9</xdr:col>
-      <xdr:colOff>714375</xdr:colOff>
+      <xdr:colOff>200025</xdr:colOff>
       <xdr:row>38</xdr:row>
-      <xdr:rowOff>114300</xdr:rowOff>
+      <xdr:rowOff>138010</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
-        <xdr:cNvPr id="4" name="Picture 3"/>
+        <xdr:cNvPr id="3" name="Picture 2"/>
         <xdr:cNvPicPr>
           <a:picLocks noChangeAspect="1" noChangeArrowheads="1"/>
         </xdr:cNvPicPr>
@@ -455,7 +455,7 @@
       <xdr:spPr bwMode="auto">
         <a:xfrm>
           <a:off x="1009650" y="809625"/>
-          <a:ext cx="8791575" cy="6781800"/>
+          <a:ext cx="8277225" cy="6805510"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -488,13 +488,13 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>9</xdr:col>
-      <xdr:colOff>619125</xdr:colOff>
-      <xdr:row>41</xdr:row>
-      <xdr:rowOff>47625</xdr:rowOff>
+      <xdr:colOff>628650</xdr:colOff>
+      <xdr:row>37</xdr:row>
+      <xdr:rowOff>133350</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
-        <xdr:cNvPr id="4" name="Picture 3"/>
+        <xdr:cNvPr id="3" name="Picture 2"/>
         <xdr:cNvPicPr>
           <a:picLocks noChangeAspect="1" noChangeArrowheads="1"/>
         </xdr:cNvPicPr>
@@ -515,7 +515,7 @@
       <xdr:spPr bwMode="auto">
         <a:xfrm>
           <a:off x="1009650" y="809625"/>
-          <a:ext cx="8696325" cy="7286625"/>
+          <a:ext cx="8705850" cy="6610350"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -816,26 +816,26 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:11" s="2" customFormat="1" ht="25.5" x14ac:dyDescent="0.25">
-      <c r="A1" s="19" t="s">
+      <c r="A1" s="20" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="19"/>
-      <c r="C1" s="19"/>
-      <c r="D1" s="19"/>
-      <c r="E1" s="19"/>
-      <c r="F1" s="19"/>
-      <c r="G1" s="19"/>
-      <c r="H1" s="19"/>
-      <c r="I1" s="19"/>
-      <c r="J1" s="19"/>
+      <c r="B1" s="20"/>
+      <c r="C1" s="20"/>
+      <c r="D1" s="20"/>
+      <c r="E1" s="20"/>
+      <c r="F1" s="20"/>
+      <c r="G1" s="20"/>
+      <c r="H1" s="20"/>
+      <c r="I1" s="20"/>
+      <c r="J1" s="20"/>
       <c r="K1" s="1"/>
     </row>
     <row r="2" spans="1:11" s="2" customFormat="1" ht="25.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A2" s="20" t="s">
+      <c r="A2" s="21" t="s">
         <v>1</v>
       </c>
-      <c r="B2" s="20"/>
-      <c r="C2" s="20"/>
+      <c r="B2" s="21"/>
+      <c r="C2" s="21"/>
       <c r="D2" s="3"/>
       <c r="E2" s="3"/>
       <c r="F2" s="3"/>
@@ -849,205 +849,237 @@
       <c r="A3" s="5" t="s">
         <v>2</v>
       </c>
-      <c r="B3" s="21" t="s">
+      <c r="B3" s="22" t="s">
         <v>3</v>
       </c>
-      <c r="C3" s="21"/>
-      <c r="D3" s="21"/>
-      <c r="E3" s="21" t="s">
+      <c r="C3" s="22"/>
+      <c r="D3" s="22"/>
+      <c r="E3" s="22" t="s">
         <v>4</v>
       </c>
-      <c r="F3" s="21"/>
-      <c r="G3" s="21" t="s">
+      <c r="F3" s="22"/>
+      <c r="G3" s="22" t="s">
         <v>5</v>
       </c>
-      <c r="H3" s="21"/>
-      <c r="I3" s="21"/>
-      <c r="J3" s="21"/>
-      <c r="K3" s="21"/>
+      <c r="H3" s="22"/>
+      <c r="I3" s="22"/>
+      <c r="J3" s="22"/>
+      <c r="K3" s="22"/>
     </row>
     <row r="4" spans="1:11" ht="42.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A4" s="7">
         <v>1</v>
       </c>
-      <c r="B4" s="17" t="s">
+      <c r="B4" s="19" t="s">
         <v>12</v>
       </c>
-      <c r="C4" s="18"/>
-      <c r="D4" s="18"/>
-      <c r="E4" s="18" t="s">
+      <c r="C4" s="17"/>
+      <c r="D4" s="17"/>
+      <c r="E4" s="17" t="s">
         <v>6</v>
       </c>
-      <c r="F4" s="18"/>
-      <c r="G4" s="18" t="s">
+      <c r="F4" s="17"/>
+      <c r="G4" s="17" t="s">
         <v>7</v>
       </c>
-      <c r="H4" s="18"/>
-      <c r="I4" s="18"/>
-      <c r="J4" s="18"/>
-      <c r="K4" s="18"/>
+      <c r="H4" s="17"/>
+      <c r="I4" s="17"/>
+      <c r="J4" s="17"/>
+      <c r="K4" s="17"/>
     </row>
     <row r="5" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A5" s="7">
         <v>2</v>
       </c>
-      <c r="B5" s="18" t="s">
+      <c r="B5" s="17" t="s">
         <v>13</v>
       </c>
-      <c r="C5" s="18"/>
-      <c r="D5" s="18"/>
-      <c r="E5" s="22">
+      <c r="C5" s="17"/>
+      <c r="D5" s="17"/>
+      <c r="E5" s="18">
         <v>42825</v>
       </c>
-      <c r="F5" s="18"/>
-      <c r="G5" s="18" t="s">
+      <c r="F5" s="17"/>
+      <c r="G5" s="17" t="s">
         <v>14</v>
       </c>
-      <c r="H5" s="18"/>
-      <c r="I5" s="18"/>
-      <c r="J5" s="18"/>
-      <c r="K5" s="18"/>
+      <c r="H5" s="17"/>
+      <c r="I5" s="17"/>
+      <c r="J5" s="17"/>
+      <c r="K5" s="17"/>
     </row>
     <row r="6" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A6" s="7">
         <v>3</v>
       </c>
-      <c r="B6" s="18" t="s">
+      <c r="B6" s="17" t="s">
         <v>13</v>
       </c>
-      <c r="C6" s="18"/>
-      <c r="D6" s="18"/>
-      <c r="E6" s="22">
+      <c r="C6" s="17"/>
+      <c r="D6" s="17"/>
+      <c r="E6" s="18">
         <v>42828</v>
       </c>
-      <c r="F6" s="18"/>
-      <c r="G6" s="18" t="s">
+      <c r="F6" s="17"/>
+      <c r="G6" s="17" t="s">
         <v>15</v>
       </c>
-      <c r="H6" s="18"/>
-      <c r="I6" s="18"/>
-      <c r="J6" s="18"/>
-      <c r="K6" s="18"/>
+      <c r="H6" s="17"/>
+      <c r="I6" s="17"/>
+      <c r="J6" s="17"/>
+      <c r="K6" s="17"/>
     </row>
     <row r="7" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A7" s="7"/>
-      <c r="B7" s="18"/>
-      <c r="C7" s="18"/>
-      <c r="D7" s="18"/>
-      <c r="E7" s="18"/>
-      <c r="F7" s="18"/>
-      <c r="G7" s="18"/>
-      <c r="H7" s="18"/>
-      <c r="I7" s="18"/>
-      <c r="J7" s="18"/>
-      <c r="K7" s="18"/>
+      <c r="B7" s="17"/>
+      <c r="C7" s="17"/>
+      <c r="D7" s="17"/>
+      <c r="E7" s="17"/>
+      <c r="F7" s="17"/>
+      <c r="G7" s="17"/>
+      <c r="H7" s="17"/>
+      <c r="I7" s="17"/>
+      <c r="J7" s="17"/>
+      <c r="K7" s="17"/>
     </row>
     <row r="8" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A8" s="7"/>
-      <c r="B8" s="18"/>
-      <c r="C8" s="18"/>
-      <c r="D8" s="18"/>
-      <c r="E8" s="18"/>
-      <c r="F8" s="18"/>
-      <c r="G8" s="18"/>
-      <c r="H8" s="18"/>
-      <c r="I8" s="18"/>
-      <c r="J8" s="18"/>
-      <c r="K8" s="18"/>
+      <c r="B8" s="17"/>
+      <c r="C8" s="17"/>
+      <c r="D8" s="17"/>
+      <c r="E8" s="17"/>
+      <c r="F8" s="17"/>
+      <c r="G8" s="17"/>
+      <c r="H8" s="17"/>
+      <c r="I8" s="17"/>
+      <c r="J8" s="17"/>
+      <c r="K8" s="17"/>
     </row>
     <row r="9" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A9" s="7"/>
-      <c r="B9" s="18"/>
-      <c r="C9" s="18"/>
-      <c r="D9" s="18"/>
-      <c r="E9" s="18"/>
-      <c r="F9" s="18"/>
-      <c r="G9" s="18"/>
-      <c r="H9" s="18"/>
-      <c r="I9" s="18"/>
-      <c r="J9" s="18"/>
-      <c r="K9" s="18"/>
+      <c r="B9" s="17"/>
+      <c r="C9" s="17"/>
+      <c r="D9" s="17"/>
+      <c r="E9" s="17"/>
+      <c r="F9" s="17"/>
+      <c r="G9" s="17"/>
+      <c r="H9" s="17"/>
+      <c r="I9" s="17"/>
+      <c r="J9" s="17"/>
+      <c r="K9" s="17"/>
     </row>
     <row r="10" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A10" s="7"/>
-      <c r="B10" s="18"/>
-      <c r="C10" s="18"/>
-      <c r="D10" s="18"/>
-      <c r="E10" s="18"/>
-      <c r="F10" s="18"/>
-      <c r="G10" s="18"/>
-      <c r="H10" s="18"/>
-      <c r="I10" s="18"/>
-      <c r="J10" s="18"/>
-      <c r="K10" s="18"/>
+      <c r="B10" s="17"/>
+      <c r="C10" s="17"/>
+      <c r="D10" s="17"/>
+      <c r="E10" s="17"/>
+      <c r="F10" s="17"/>
+      <c r="G10" s="17"/>
+      <c r="H10" s="17"/>
+      <c r="I10" s="17"/>
+      <c r="J10" s="17"/>
+      <c r="K10" s="17"/>
     </row>
     <row r="11" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A11" s="7"/>
-      <c r="B11" s="18"/>
-      <c r="C11" s="18"/>
-      <c r="D11" s="18"/>
-      <c r="E11" s="18"/>
-      <c r="F11" s="18"/>
-      <c r="G11" s="18"/>
-      <c r="H11" s="18"/>
-      <c r="I11" s="18"/>
-      <c r="J11" s="18"/>
-      <c r="K11" s="18"/>
+      <c r="B11" s="17"/>
+      <c r="C11" s="17"/>
+      <c r="D11" s="17"/>
+      <c r="E11" s="17"/>
+      <c r="F11" s="17"/>
+      <c r="G11" s="17"/>
+      <c r="H11" s="17"/>
+      <c r="I11" s="17"/>
+      <c r="J11" s="17"/>
+      <c r="K11" s="17"/>
     </row>
     <row r="12" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A12" s="7"/>
-      <c r="B12" s="18"/>
-      <c r="C12" s="18"/>
-      <c r="D12" s="18"/>
-      <c r="E12" s="18"/>
-      <c r="F12" s="18"/>
-      <c r="G12" s="18"/>
-      <c r="H12" s="18"/>
-      <c r="I12" s="18"/>
-      <c r="J12" s="18"/>
-      <c r="K12" s="18"/>
+      <c r="B12" s="17"/>
+      <c r="C12" s="17"/>
+      <c r="D12" s="17"/>
+      <c r="E12" s="17"/>
+      <c r="F12" s="17"/>
+      <c r="G12" s="17"/>
+      <c r="H12" s="17"/>
+      <c r="I12" s="17"/>
+      <c r="J12" s="17"/>
+      <c r="K12" s="17"/>
     </row>
     <row r="13" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A13" s="7"/>
-      <c r="B13" s="18"/>
-      <c r="C13" s="18"/>
-      <c r="D13" s="18"/>
-      <c r="E13" s="18"/>
-      <c r="F13" s="18"/>
-      <c r="G13" s="18"/>
-      <c r="H13" s="18"/>
-      <c r="I13" s="18"/>
-      <c r="J13" s="18"/>
-      <c r="K13" s="18"/>
+      <c r="B13" s="17"/>
+      <c r="C13" s="17"/>
+      <c r="D13" s="17"/>
+      <c r="E13" s="17"/>
+      <c r="F13" s="17"/>
+      <c r="G13" s="17"/>
+      <c r="H13" s="17"/>
+      <c r="I13" s="17"/>
+      <c r="J13" s="17"/>
+      <c r="K13" s="17"/>
     </row>
     <row r="14" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A14" s="7"/>
-      <c r="B14" s="18"/>
-      <c r="C14" s="18"/>
-      <c r="D14" s="18"/>
-      <c r="E14" s="18"/>
-      <c r="F14" s="18"/>
-      <c r="G14" s="18"/>
-      <c r="H14" s="18"/>
-      <c r="I14" s="18"/>
-      <c r="J14" s="18"/>
-      <c r="K14" s="18"/>
+      <c r="B14" s="17"/>
+      <c r="C14" s="17"/>
+      <c r="D14" s="17"/>
+      <c r="E14" s="17"/>
+      <c r="F14" s="17"/>
+      <c r="G14" s="17"/>
+      <c r="H14" s="17"/>
+      <c r="I14" s="17"/>
+      <c r="J14" s="17"/>
+      <c r="K14" s="17"/>
     </row>
     <row r="15" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A15" s="7"/>
-      <c r="B15" s="18"/>
-      <c r="C15" s="18"/>
-      <c r="D15" s="18"/>
-      <c r="E15" s="18"/>
-      <c r="F15" s="18"/>
-      <c r="G15" s="18"/>
-      <c r="H15" s="18"/>
-      <c r="I15" s="18"/>
-      <c r="J15" s="18"/>
-      <c r="K15" s="18"/>
+      <c r="B15" s="17"/>
+      <c r="C15" s="17"/>
+      <c r="D15" s="17"/>
+      <c r="E15" s="17"/>
+      <c r="F15" s="17"/>
+      <c r="G15" s="17"/>
+      <c r="H15" s="17"/>
+      <c r="I15" s="17"/>
+      <c r="J15" s="17"/>
+      <c r="K15" s="17"/>
     </row>
   </sheetData>
   <mergeCells count="41">
+    <mergeCell ref="B4:D4"/>
+    <mergeCell ref="E4:F4"/>
+    <mergeCell ref="G4:K4"/>
+    <mergeCell ref="A1:J1"/>
+    <mergeCell ref="A2:C2"/>
+    <mergeCell ref="B3:D3"/>
+    <mergeCell ref="E3:F3"/>
+    <mergeCell ref="G3:K3"/>
+    <mergeCell ref="B5:D5"/>
+    <mergeCell ref="E5:F5"/>
+    <mergeCell ref="G5:K5"/>
+    <mergeCell ref="B6:D6"/>
+    <mergeCell ref="E6:F6"/>
+    <mergeCell ref="G6:K6"/>
+    <mergeCell ref="B7:D7"/>
+    <mergeCell ref="E7:F7"/>
+    <mergeCell ref="G7:K7"/>
+    <mergeCell ref="B8:D8"/>
+    <mergeCell ref="E8:F8"/>
+    <mergeCell ref="G8:K8"/>
+    <mergeCell ref="B9:D9"/>
+    <mergeCell ref="E9:F9"/>
+    <mergeCell ref="G9:K9"/>
+    <mergeCell ref="B10:D10"/>
+    <mergeCell ref="E10:F10"/>
+    <mergeCell ref="G10:K10"/>
+    <mergeCell ref="B11:D11"/>
+    <mergeCell ref="E11:F11"/>
+    <mergeCell ref="G11:K11"/>
+    <mergeCell ref="B12:D12"/>
+    <mergeCell ref="E12:F12"/>
+    <mergeCell ref="G12:K12"/>
     <mergeCell ref="B15:D15"/>
     <mergeCell ref="E15:F15"/>
     <mergeCell ref="G15:K15"/>
@@ -1057,38 +1089,6 @@
     <mergeCell ref="B14:D14"/>
     <mergeCell ref="E14:F14"/>
     <mergeCell ref="G14:K14"/>
-    <mergeCell ref="B11:D11"/>
-    <mergeCell ref="E11:F11"/>
-    <mergeCell ref="G11:K11"/>
-    <mergeCell ref="B12:D12"/>
-    <mergeCell ref="E12:F12"/>
-    <mergeCell ref="G12:K12"/>
-    <mergeCell ref="B9:D9"/>
-    <mergeCell ref="E9:F9"/>
-    <mergeCell ref="G9:K9"/>
-    <mergeCell ref="B10:D10"/>
-    <mergeCell ref="E10:F10"/>
-    <mergeCell ref="G10:K10"/>
-    <mergeCell ref="B7:D7"/>
-    <mergeCell ref="E7:F7"/>
-    <mergeCell ref="G7:K7"/>
-    <mergeCell ref="B8:D8"/>
-    <mergeCell ref="E8:F8"/>
-    <mergeCell ref="G8:K8"/>
-    <mergeCell ref="B5:D5"/>
-    <mergeCell ref="E5:F5"/>
-    <mergeCell ref="G5:K5"/>
-    <mergeCell ref="B6:D6"/>
-    <mergeCell ref="E6:F6"/>
-    <mergeCell ref="G6:K6"/>
-    <mergeCell ref="B4:D4"/>
-    <mergeCell ref="E4:F4"/>
-    <mergeCell ref="G4:K4"/>
-    <mergeCell ref="A1:J1"/>
-    <mergeCell ref="A2:C2"/>
-    <mergeCell ref="B3:D3"/>
-    <mergeCell ref="E3:F3"/>
-    <mergeCell ref="G3:K3"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -1099,7 +1099,7 @@
   <dimension ref="A1:AQ130"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B4" sqref="B4"/>
+      <selection activeCell="J36" sqref="J36"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="15.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2786,7 +2786,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:AS137"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView tabSelected="1" topLeftCell="A13" workbookViewId="0">
       <selection activeCell="B4" sqref="B4"/>
     </sheetView>
   </sheetViews>

</xml_diff>